<commit_message>
V2 du fichier pense-bête
</commit_message>
<xml_diff>
--- a/Git débutant (Pense-bête).xlsx
+++ b/Git débutant (Pense-bête).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14640" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="20320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
   <si>
     <t>Commande</t>
   </si>
@@ -164,9 +164,6 @@
     <t>Quand ça va mal</t>
   </si>
   <si>
-    <t>Enlève le fichier de la liste des fichiers à consigner</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">git clone </t>
     </r>
@@ -282,6 +279,99 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">git tag étiquette </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>NuméroDeConsigne</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Pose une étiquette après coup sur la consigne numéro </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>NuméroDeConsigne</t>
+    </r>
+  </si>
+  <si>
+    <t>git commit --amend</t>
+  </si>
+  <si>
+    <t>Pour ajouter des fichiers à la consigne ou pour modifier le message de consigne</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git reset HEAD </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>fichier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Enlève le</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve"> fichier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve"> du dépôt</t>
+    </r>
+  </si>
+  <si>
+    <t>Contexte : 1 dépôt sur GitHub, 1 seul développeur, 0 branches. On reste dans la simplicité.</t>
+  </si>
+  <si>
+    <t>git config --global user.name NomUtilisateur</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git remote add origin </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>serveur</t>
+    </r>
+  </si>
+  <si>
+    <t>Connecte le dépôt local au dépôt distant principal (serveur)</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">git push origin </t>
     </r>
     <r>
@@ -289,8 +379,7 @@
         <i/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
+        <rFont val="Avenir Next Regular"/>
       </rPr>
       <t>étiquette</t>
     </r>
@@ -304,8 +393,7 @@
         <i/>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
+        <rFont val="Avenir Next Regular"/>
       </rPr>
       <t>modifications étiquettées</t>
     </r>
@@ -313,50 +401,14 @@
       <rPr>
         <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
+        <rFont val="Avenir Next Regular"/>
       </rPr>
       <t xml:space="preserve"> sur le dépôt principal</t>
     </r>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">git tag étiquette </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Avenir Next Regular"/>
-      </rPr>
-      <t>NuméroDeConsigne</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Pose une étiquette après coup sur la consigne numéro </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Avenir Next Regular"/>
-      </rPr>
-      <t>NuméroDeConsigne</t>
-    </r>
-  </si>
-  <si>
-    <t>git commit --amend</t>
-  </si>
-  <si>
-    <t>Pour ajouter des fichiers à la consigne ou pour modifier le message de consigne</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">git reset HEAD </t>
+      <t xml:space="preserve">Enlève le </t>
     </r>
     <r>
       <rPr>
@@ -367,41 +419,21 @@
       </rPr>
       <t>fichier</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t>Enlève le</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Avenir Next Regular"/>
-      </rPr>
-      <t xml:space="preserve"> fichier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Avenir Next Regular"/>
-      </rPr>
-      <t xml:space="preserve"> du dépôt</t>
-    </r>
-  </si>
-  <si>
-    <t>Contexte : 1 dépôt sur GitHub, 1 seul développeur, 0 branches. On reste dans la simplicité.</t>
-  </si>
-  <si>
-    <t>git config --global user.name NomUtilisateur</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve"> de la liste des fichiers à consigner</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -476,31 +508,17 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="8"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
+      <name val="Avenir Next Regular"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor theme="0" tint="-0.14999847407452621"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -510,19 +528,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.34998626667073579"/>
+        <fgColor theme="0"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF595959"/>
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor theme="0" tint="-0.14999847407452621"/>
       </patternFill>
     </fill>
@@ -536,7 +578,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -556,8 +598,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -565,25 +609,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -591,8 +628,21 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -602,6 +652,7 @@
     <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -611,6 +662,7 @@
     <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1112,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A20" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1127,15 +1179,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="33" customHeight="1">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="12" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="12"/>
+      <c r="E1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="15">
       <c r="A2" s="4" t="s">
@@ -1153,147 +1205,151 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="37" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="C3" s="7"/>
+    </row>
+    <row r="4" spans="1:5" ht="37" customHeight="1">
+      <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" ht="37" customHeight="1">
-      <c r="A4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="5"/>
+      <c r="D4" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="37" customHeight="1">
+      <c r="A5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="37" customHeight="1">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="37" customHeight="1">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="37" customHeight="1">
+      <c r="A8" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="37" customHeight="1">
+      <c r="A9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="37" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="37" customHeight="1">
-      <c r="A6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="37" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="E9" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="37" customHeight="1">
+      <c r="A10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" ht="15">
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="14" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="37" customHeight="1">
-      <c r="A8" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="37" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="37" customHeight="1">
-      <c r="A10" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" spans="1:5" ht="15">
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" spans="1:5" ht="15">
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" ht="15">
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" ht="15">
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-    </row>
-    <row r="15" spans="1:5" ht="15">
-      <c r="A15" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
     </row>
     <row r="16" spans="1:5" ht="15">
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
     </row>
     <row r="17" spans="1:5" ht="15">
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="19" spans="1:5" ht="33" customHeight="1">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="7"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:5" ht="15">
       <c r="A20" s="4" t="s">
@@ -1305,55 +1361,55 @@
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:5" ht="37" customHeight="1">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="7"/>
     </row>
     <row r="22" spans="1:5" ht="37" customHeight="1">
-      <c r="A22" s="6" t="s">
+      <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="37" customHeight="1">
-      <c r="A23" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" s="5" t="s">
+      <c r="A23" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="7"/>
     </row>
     <row r="24" spans="1:5" ht="37" customHeight="1">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="37" customHeight="1">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="8"/>
+      <c r="A25" s="13"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:5" ht="37" customHeight="1">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:5" ht="37" customHeight="1">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="8"/>
+      <c r="A27" s="13"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1365,8 +1421,8 @@
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
-    <oddHeader>&amp;C&amp;"Calibri,Normal"&amp;K000000Git pour les débutants&amp;R&amp;"Calibri,Normal"&amp;K000000&amp;P/&amp;N</oddHeader>
-    <oddFooter>&amp;L&amp;"Calibri,Normal"&amp;K000000&amp;F&amp;R&amp;"Calibri,Normal"&amp;K000000&amp;D</oddFooter>
+    <oddHeader>&amp;C&amp;"Avenir Next Regular,Normal"&amp;8&amp;K000000Git pour les débutants&amp;R&amp;"Avenir Next Regular,Normal"&amp;8&amp;K000000&amp;P/&amp;N</oddHeader>
+    <oddFooter>&amp;L&amp;"Avenir Next Regular,Normal"&amp;8&amp;K000000&amp;F&amp;R&amp;"Avenir Next Regular,Normal"&amp;8&amp;K000000&amp;D</oddFooter>
   </headerFooter>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
V3 du fichier pense-bête.
</commit_message>
<xml_diff>
--- a/Git débutant (Pense-bête).xlsx
+++ b/Git débutant (Pense-bête).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="20320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="20320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>Commande</t>
   </si>
@@ -164,13 +164,28 @@
     <t>Quand ça va mal</t>
   </si>
   <si>
+    <t>git commit --amend</t>
+  </si>
+  <si>
+    <t>Pour ajouter des fichiers à la consigne ou pour modifier le message de consigne</t>
+  </si>
+  <si>
+    <t>Contexte : 1 dépôt sur GitHub, 1 seul développeur, 0 branches. On reste dans la simplicité.</t>
+  </si>
+  <si>
+    <t>git config --global user.name NomUtilisateur</t>
+  </si>
+  <si>
+    <t>Connecte le dépôt local au dépôt distant principal (serveur)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">git clone </t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -184,7 +199,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -198,7 +213,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -212,7 +227,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -220,7 +235,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -234,7 +249,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -243,12 +258,70 @@
   </si>
   <si>
     <r>
+      <t>Enlève le</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve"> fichier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve"> du dépôt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git reset HEAD </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>fichier</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Enlève le </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>fichier</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve"> de la liste des fichiers à consigner</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">git tag </t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -262,7 +335,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -270,7 +343,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -284,7 +357,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -298,7 +371,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -306,61 +379,13 @@
     </r>
   </si>
   <si>
-    <t>git commit --amend</t>
-  </si>
-  <si>
-    <t>Pour ajouter des fichiers à la consigne ou pour modifier le message de consigne</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">git reset HEAD </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Avenir Next Regular"/>
-      </rPr>
-      <t>fichier</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Enlève le</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Avenir Next Regular"/>
-      </rPr>
-      <t xml:space="preserve"> fichier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Avenir Next Regular"/>
-      </rPr>
-      <t xml:space="preserve"> du dépôt</t>
-    </r>
-  </si>
-  <si>
-    <t>Contexte : 1 dépôt sur GitHub, 1 seul développeur, 0 branches. On reste dans la simplicité.</t>
-  </si>
-  <si>
-    <t>git config --global user.name NomUtilisateur</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">git remote add origin </t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -368,16 +393,13 @@
     </r>
   </si>
   <si>
-    <t>Connecte le dépôt local au dépôt distant principal (serveur)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">git push origin </t>
     </r>
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -391,7 +413,7 @@
     <r>
       <rPr>
         <i/>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -399,7 +421,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="10"/>
+        <sz val="8"/>
         <color theme="1"/>
         <rFont val="Avenir Next Regular"/>
       </rPr>
@@ -407,33 +429,189 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Enlève le </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Avenir Next Regular"/>
-      </rPr>
-      <t>fichier</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Avenir Next Regular"/>
-      </rPr>
-      <t xml:space="preserve"> de la liste des fichiers à consigner</t>
-    </r>
+    <t>1. Aller sur le site GitHub.</t>
+  </si>
+  <si>
+    <t>2. Créer un compte :</t>
+  </si>
+  <si>
+    <t>3. Créer un dépôt : Create a repository :</t>
+  </si>
+  <si>
+    <t>Créer un dépôt sur le site GitHub (www.github.com)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    2.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>Pick a username</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>: choisissez un nom d'utilisateur.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    2.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve">Your email </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>: entrez votre adresse mail.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    2.3 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve">Create a password </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>: entrez votre mot de passe</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    2.4 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve">Sign up for GitHub </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>: cliquez sur le bouton pour vous enregistrer.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    3.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve">Repository name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>: entrez un nom pour votre dépôt.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    3.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve">Description </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>: entrez une description de ce que contient votre dépôt.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    3.3 </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve">Public </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>: cocher publique (un dépôt privé est payant).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    3.4 Initialize</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve"> this repository with a README</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t xml:space="preserve">: cochez "​initialiser le dépôt avec un fichier lisezmoit.txt​" pour ajouter un fichier readme.md comme premier fichier du dépôt. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">    Ce fichier servira à décrire en détail le contenu du dépôt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3.5 Create a repository : cliquez sur le bouton "​Créer un dépôt". </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -471,18 +649,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="0"/>
-      <name val="Avenir Next Regular"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Avenir Next Regular"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -490,18 +656,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Avenir Next Regular"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Avenir Next Regular"/>
-    </font>
-    <font>
-      <i/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Avenir Next Regular"/>
@@ -510,6 +664,45 @@
       <b/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Avenir Next Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0"/>
+      <name val="Avenir Next Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Avenir Next Regular"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Avenir Next Regular"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Avenir Next Regular"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Avenir Next Regular"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8"/>
       <name val="Avenir Next Regular"/>
     </font>
   </fonts>
@@ -578,7 +771,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -600,8 +793,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -609,40 +808,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="27">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
@@ -653,6 +858,9 @@
     <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
@@ -663,6 +871,9 @@
     <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -1162,260 +1373,317 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="2.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38" style="3" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="13.1640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="28" style="3" customWidth="1"/>
+    <col min="3" max="3" width="1" style="3" customWidth="1"/>
+    <col min="4" max="4" width="13.1640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="28" style="3" customWidth="1"/>
+    <col min="6" max="6" width="1" style="3" customWidth="1"/>
+    <col min="7" max="7" width="14" style="3" customWidth="1"/>
+    <col min="8" max="8" width="23" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="33" customHeight="1">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" ht="33" customHeight="1">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" s="4" t="s">
+      <c r="E1" s="8"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="37" customHeight="1">
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="37" customHeight="1">
       <c r="A3" s="10" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="7"/>
-    </row>
-    <row r="4" spans="1:5" ht="37" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="37" customHeight="1">
+        <v>34</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="37" customHeight="1">
+      <c r="A4" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="37" customHeight="1">
       <c r="A5" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5" t="s">
+      <c r="C5" s="11"/>
+      <c r="D5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="37" customHeight="1">
-      <c r="A6" s="5" t="s">
+      <c r="E5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="11"/>
+      <c r="G5" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="37" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="11" t="s">
+      <c r="C6" s="13"/>
+      <c r="D6" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="37" customHeight="1">
+      <c r="F6" s="13"/>
+      <c r="G6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="37" customHeight="1">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="37" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="37" customHeight="1">
+      <c r="C7" s="11"/>
+      <c r="D7" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+    </row>
+    <row r="8" spans="1:8" ht="37" customHeight="1">
+      <c r="A8" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="13"/>
+      <c r="D8" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+    </row>
+    <row r="9" spans="1:8" ht="37" customHeight="1">
       <c r="A9" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="37" customHeight="1">
-      <c r="A10" s="7" t="s">
+      <c r="C9" s="11"/>
+      <c r="D9" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="E9" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="11"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+    </row>
+    <row r="10" spans="1:8" ht="37" customHeight="1">
+      <c r="A10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" ht="15">
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-    </row>
-    <row r="12" spans="1:5" ht="15">
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" ht="15">
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:5" ht="15">
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-    </row>
-    <row r="15" spans="1:5" ht="15">
-      <c r="A15" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" ht="15">
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" ht="15">
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="19" spans="1:5" ht="33" customHeight="1">
-      <c r="A19" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="12"/>
-      <c r="C19" s="6"/>
-    </row>
-    <row r="20" spans="1:5" ht="15">
-      <c r="A20" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4"/>
-    </row>
-    <row r="21" spans="1:5" ht="37" customHeight="1">
-      <c r="A21" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" ht="37" customHeight="1">
-      <c r="A22" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:5" ht="37" customHeight="1">
-      <c r="A23" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="7"/>
-    </row>
-    <row r="24" spans="1:5" ht="37" customHeight="1">
-      <c r="A24" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:5" ht="37" customHeight="1">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" ht="37" customHeight="1">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:5" ht="37" customHeight="1">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="7"/>
+      <c r="B10" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" spans="1:8" ht="15">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="15">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:8" ht="15">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="15">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="15">
+      <c r="A15" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="18" spans="1:5" ht="15">
+      <c r="A18" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="17" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A19:B19"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Ajout de git checkout.
</commit_message>
<xml_diff>
--- a/Git débutant (Pense-bête).xlsx
+++ b/Git débutant (Pense-bête).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27600" windowHeight="20320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3120" yWindow="80" windowWidth="27600" windowHeight="20320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>Commande</t>
   </si>
@@ -605,6 +605,51 @@
   </si>
   <si>
     <t xml:space="preserve">    3.5 Create a repository : cliquez sur le bouton "​Créer un dépôt". </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git  checkout        </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>N° de commit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Revient à l'état du commit </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>N° de commit</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">git checkout </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Avenir Next Regular"/>
+      </rPr>
+      <t>master</t>
+    </r>
+  </si>
+  <si>
+    <t>Revient à l'état du dernier commit</t>
   </si>
 </sst>
 </file>
@@ -813,13 +858,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -838,14 +877,20 @@
     <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -1375,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A12" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="149" zoomScaleNormal="149" zoomScalePageLayoutView="149" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1393,192 +1438,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="15" t="s">
+      <c r="E1" s="17"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="15"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="37" customHeight="1">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="16" t="s">
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="37" customHeight="1">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="11"/>
+      <c r="D4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="11" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="37" customHeight="1">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="13" t="s">
+      <c r="C5" s="9"/>
+      <c r="D5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="9"/>
+      <c r="G5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="37" customHeight="1">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="14" t="s">
+      <c r="C6" s="11"/>
+      <c r="D6" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
+      <c r="F6" s="11"/>
+      <c r="G6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="13" t="s">
+      <c r="H6" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="37" customHeight="1">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="37" customHeight="1">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="14" t="s">
+      <c r="C8" s="11"/>
+      <c r="D8" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="37" customHeight="1">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="13" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" ht="37" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10"/>
     </row>
     <row r="11" spans="1:8" ht="15">
       <c r="D11" s="4"/>
@@ -1615,67 +1668,67 @@
       <c r="E18" s="4"/>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="15" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="15" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="15" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="15" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="15" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="15" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="15" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="14" t="s">
         <v>61</v>
       </c>
     </row>

</xml_diff>